<commit_message>
Working on multiple things
-trying to get the event-driven simulation to work for case_study_4.2
-Added scripts to display CSS information
</commit_message>
<xml_diff>
--- a/6_publication/1_toPSAil/1_plots/8.0_css_comparisons/kayser_css_comparison_data_2022_12_22_v1.xlsx
+++ b/6_publication/1_toPSAil/1_plots/8.0_css_comparisons/kayser_css_comparison_data_2022_12_22_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkim333\Documents\GitHub\toPSAil\6_publication\1_toPSAil\1_plots\8.0_css_comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5913051F-C2AB-4A9F-B97C-F16A3BE6C23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802E216C-FC6E-42BD-A98B-28C39CF7C1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{EAFE1014-9F5F-4131-970F-58F315BD01A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{EAFE1014-9F5F-4131-970F-58F315BD01A8}"/>
   </bookViews>
   <sheets>
     <sheet name="kayser (flow+time)" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'kayser (flow+event)'!$B$2:$K$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'kayser (flow+time)'!$B$2:$K$30</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'kayser (pres.+event)'!$B$2:$K$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'kayser (pres.+event)'!$B$2:$K$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'kayser (pres.+time)'!$B$2:$K$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -780,22 +780,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.5779141105123101E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.1024417699829603E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.2068579208866E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.0258892967883001E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6.07355146616586E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -995,7 +992,7 @@
         <c:axId val="454142080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="7"/>
+          <c:max val="6"/>
           <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2213,7 +2210,7 @@
   <dimension ref="C4:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D10" sqref="C5:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2432,7 +2429,7 @@
   <dimension ref="C4:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2634,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FAD013-A2F7-42D1-AF99-AD6B29236AE0}">
   <dimension ref="C4:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2843,10 +2840,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9269801-6C6F-463A-B27E-A31CD8816D0C}">
-  <dimension ref="C4:H18"/>
+  <dimension ref="C4:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F17"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2868,146 +2865,182 @@
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.5779141105123101E-2</v>
+      </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6.1024417699829603E-5</v>
+      </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.2068579208866E-6</v>
+      </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3.0258892967883001E-8</v>
+      </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6.07355146616586E-9</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2">
+        <v>113.453</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1E-8</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
         <v>2</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>5</v>
+      <c r="H12" s="4">
+        <f>D12/(F12*G12)</f>
+        <v>11.3453</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>110.14100000000001</v>
+      </c>
       <c r="E13" s="3">
         <v>1E-8</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
       <c r="G13" s="2">
         <v>2</v>
       </c>
-      <c r="H13" s="4" t="e">
-        <f>D13/(F13*G13)</f>
-        <v>#DIV/0!</v>
+      <c r="H13" s="4">
+        <f t="shared" ref="H13:H16" si="0">D13/(F13*G13)</f>
+        <v>11.014100000000001</v>
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>113.10899999999999</v>
+      </c>
       <c r="E14" s="3">
         <v>1E-8</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
       <c r="G14" s="2">
         <v>2</v>
       </c>
-      <c r="H14" s="4" t="e">
-        <f t="shared" ref="H14:H17" si="0">D14/(F14*G14)</f>
-        <v>#DIV/0!</v>
+      <c r="H14" s="4">
+        <f t="shared" si="0"/>
+        <v>11.3109</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D15" s="2">
+        <v>112.172</v>
+      </c>
       <c r="E15" s="3">
         <v>1E-8</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
       <c r="G15" s="2">
         <v>2</v>
       </c>
-      <c r="H15" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="H15" s="4">
+        <f t="shared" si="0"/>
+        <v>11.2172</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" s="1">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>127.28100000000001</v>
+      </c>
       <c r="E16" s="3">
         <v>1E-8</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
       <c r="G16" s="2">
         <v>2</v>
       </c>
-      <c r="H16" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="H16" s="4">
+        <f t="shared" si="0"/>
+        <v>12.728100000000001</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C17" s="1">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3">
-        <v>1E-8</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>2</v>
-      </c>
-      <c r="H17" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C18" s="1"/>
-      <c r="D18" s="4" t="e">
-        <f>AVERAGE(D13:D17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="4" t="e">
-        <f>AVERAGE(H13:H17)</f>
-        <v>#DIV/0!</v>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4">
+        <f>AVERAGE(D12:D16)</f>
+        <v>115.23119999999999</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="4">
+        <f>AVERAGE(H12:H16)</f>
+        <v>11.52312</v>
       </c>
     </row>
   </sheetData>
@@ -3020,8 +3053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57299F3-5F52-4C08-BAF0-A4F2DC504CBE}">
   <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3071,11 +3104,11 @@
         <v>1.5232765142272E-2</v>
       </c>
       <c r="E5" cm="1">
-        <f t="array" ref="E5:E10">'kayser (pres.+event)'!D5:D10</f>
-        <v>0</v>
+        <f t="array" ref="E5:E9">'kayser (pres.+event)'!D5:D9</f>
+        <v>1.5779141105123101E-2</v>
       </c>
       <c r="F5">
-        <f>0.00000001</f>
+        <f t="shared" ref="F5:F29" si="0">0.00000001</f>
         <v>1E-8</v>
       </c>
     </row>
@@ -3093,10 +3126,10 @@
         <v>6.15114411191518E-5</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>6.1024417699829603E-5</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F29" si="0">0.00000001</f>
+        <f t="shared" si="0"/>
         <v>1E-8</v>
       </c>
     </row>
@@ -3114,7 +3147,7 @@
         <v>1.2321222969818899E-6</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1.2068579208866E-6</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -3135,7 +3168,7 @@
         <v>2.1065195331613901E-8</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>3.0258892967883001E-8</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -3153,7 +3186,7 @@
         <v>3.1572753279198502E-9</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>6.07355146616586E-9</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -3166,9 +3199,6 @@
       </c>
       <c r="B10">
         <v>4.2192706892422999E-10</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>

</xml_diff>